<commit_message>
exercises 1 and 2 fixed, Exercise 5 solved
</commit_message>
<xml_diff>
--- a/class17/Homework/Prueba de escritorio.xlsx
+++ b/class17/Homework/Prueba de escritorio.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juansebazz/Projects/tuix/class17/Homework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F592CB10-F7DA-1848-8366-148678E9269E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AE8037-DF78-BE4F-86E5-C289476F119C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="460" windowWidth="13880" windowHeight="16800" activeTab="3" xr2:uid="{1E0E1620-C7E6-1940-823C-ACF87419C8B4}"/>
+    <workbookView xWindow="14920" yWindow="460" windowWidth="13880" windowHeight="16800" activeTab="4" xr2:uid="{1E0E1620-C7E6-1940-823C-ACF87419C8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="exercise 1" sheetId="3" r:id="rId1"/>
     <sheet name="exercise 2" sheetId="4" r:id="rId2"/>
     <sheet name="exercise 3" sheetId="1" r:id="rId3"/>
     <sheet name="exercise 4" sheetId="2" r:id="rId4"/>
+    <sheet name="exercise 5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="68">
   <si>
     <t>row</t>
   </si>
@@ -175,6 +176,69 @@
   </si>
   <si>
     <t>´ ´*********</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´*´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´*´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´*´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´*´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´*´ ´´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´*´ ´´ ´´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´*´ ´´ ´´ ´´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´*´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´*´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´*</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´**</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´***</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´***´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´***´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´***´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´***´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´***´ ´´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´***´ ´´ ´´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´***´ ´´ ´´ ´´ ´´ ´´ ´´ ´</t>
+  </si>
+  <si>
+    <t>´ ´´ ´´ ´´ ´´ ´´ ´´ ´***´ ´´ ´´ ´´ ´´ ´´ ´´ ´´ ´</t>
   </si>
 </sst>
 </file>
@@ -253,9 +317,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -263,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,7 +645,7 @@
   <dimension ref="A2:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F24"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,14 +1093,14 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="14"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1045,14 +1109,14 @@
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1">
         <v>9</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="15"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1061,14 +1125,14 @@
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1">
         <v>8</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="15"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1077,14 +1141,14 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1">
         <v>7</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="15"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1093,14 +1157,14 @@
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="15"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1109,14 +1173,14 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="1">
         <v>5</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1125,14 +1189,14 @@
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="1">
         <v>4</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="15"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1141,14 +1205,14 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="15"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1157,14 +1221,14 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="15"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1173,14 +1237,14 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1189,7 +1253,7 @@
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="1">
@@ -1198,7 +1262,7 @@
       <c r="E13" s="1">
         <v>1</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1209,14 +1273,14 @@
       <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="1">
         <v>10</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="15"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1225,14 +1289,14 @@
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1">
         <v>9</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="14"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1241,14 +1305,14 @@
       <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="1">
         <v>8</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="14"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1257,14 +1321,14 @@
       <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="1">
         <v>7</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="14"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1273,14 +1337,14 @@
       <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="1">
         <v>6</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="14"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1289,14 +1353,14 @@
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="1">
         <v>5</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="14"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1305,14 +1369,14 @@
       <c r="B20" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="14"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1321,14 +1385,14 @@
       <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="1">
         <v>3</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="14"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1337,14 +1401,14 @@
       <c r="B22" s="1">
         <v>2</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="14"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1353,7 +1417,7 @@
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D23" s="1">
@@ -1362,7 +1426,7 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="14"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1371,14 +1435,14 @@
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="14" t="s">
         <v>46</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="14" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1407,14 +1471,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1650,12 +1714,12 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
@@ -1860,7 +1924,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1897,7 +1961,7 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="1">
@@ -1913,7 +1977,7 @@
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="1">
@@ -1929,7 +1993,7 @@
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="1">
@@ -1945,7 +2009,7 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="1">
@@ -1961,7 +2025,7 @@
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="1">
@@ -1977,7 +2041,7 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="1">
@@ -1993,7 +2057,7 @@
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="1">
@@ -2009,7 +2073,7 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="1">
@@ -2025,7 +2089,7 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="1">
@@ -2041,7 +2105,7 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="1">
@@ -2059,7 +2123,7 @@
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="1"/>
@@ -2077,7 +2141,7 @@
       <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="1">
@@ -2092,7 +2156,7 @@
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="1">
@@ -2108,7 +2172,7 @@
       <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="1">
@@ -2124,7 +2188,7 @@
       <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="1">
@@ -2140,7 +2204,7 @@
       <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D18" s="1">
@@ -2156,7 +2220,7 @@
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="1">
@@ -2172,7 +2236,7 @@
       <c r="B20" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D20" s="1">
@@ -2188,7 +2252,7 @@
       <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="1">
@@ -2204,7 +2268,7 @@
       <c r="B22" s="1">
         <v>2</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="1">
@@ -2222,7 +2286,7 @@
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="1"/>
@@ -2238,7 +2302,7 @@
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="14" t="s">
         <v>35</v>
       </c>
       <c r="D24" s="1"/>
@@ -2252,7 +2316,7 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="14"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2260,7 +2324,7 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="14"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2268,7 +2332,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="14"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2276,7 +2340,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="14"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -2284,7 +2348,7 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="14"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2292,7 +2356,7 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="14"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2300,7 +2364,7 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="14"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2308,7 +2372,7 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="14"/>
+      <c r="C32" s="13"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2316,14 +2380,14 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="14"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" s="11"/>
-      <c r="C34" s="16"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="1"/>
@@ -2366,4 +2430,662 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF77297-91AD-2444-BB66-A15AC672D74E}">
+  <dimension ref="A2:G43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="38.83203125" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1">
+        <v>7</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
+        <v>8</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1">
+        <v>2</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="1">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="1">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="1">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1">
+        <v>2</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1">
+        <v>2</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1">
+        <v>3</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1">
+        <v>4</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1">
+        <v>6</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C37" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F37" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C38" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C39" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C40" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C41" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="1">
+        <v>11</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="15"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C43" s="15"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>